<commit_message>
Finalize evals for Gemma-3
</commit_message>
<xml_diff>
--- a/_data/vibe-check.xlsx
+++ b/_data/vibe-check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/1TB Home SSD/GitHub/_ statistikZH/simplify-language_cantonal-application/_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/1TB Home SSD/GitHub/_ machinelearningZH/simply-simplify-language_cantonal-application/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3455F9B3-9564-0B4F-BF5D-2BFC02F0ACAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E8E66C-AAA3-5649-9887-4D3FBA9AAEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26240" yWindow="500" windowWidth="28680" windowHeight="26000" xr2:uid="{2DB6E942-358C-824C-9323-844D7F19AA9F}"/>
+    <workbookView xWindow="10720" yWindow="500" windowWidth="31060" windowHeight="26040" xr2:uid="{2DB6E942-358C-824C-9323-844D7F19AA9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>Phi-4</t>
   </si>
@@ -163,13 +163,37 @@
   </si>
   <si>
     <t xml:space="preserve">Modell gerät in Redeschleifen. Zuviele inhaltliche und sprachliche Fehler. </t>
+  </si>
+  <si>
+    <t>QwQ 32B</t>
+  </si>
+  <si>
+    <t>Zu viele sprachliche Fehler. Kippt teils ins Englisch. Tag-Fehler, div. Ergebnisse können nicht sauber geparst werden.</t>
+  </si>
+  <si>
+    <t>Gemma 3 27B 5_K-M</t>
+  </si>
+  <si>
+    <t>Gemma 3 27B 6_K</t>
+  </si>
+  <si>
+    <t>Sehr gute Ergebnisse. Wenig inhaltliche Fehler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gute bis sehr gute Ergebnisse. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Übersetzung nah an Leichter Sprache, teils inhaltliche Missverständnisse. </t>
+  </si>
+  <si>
+    <t>Prompting scheint für Verständliche und Leichte Sprache besser zu funktionieren. Prompting muss vmtl. optimiert werden für das Modell.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,6 +220,13 @@
       <color rgb="FF000000"/>
       <name val="Aptos Display"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -260,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -323,6 +354,20 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -659,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AE979A-81C6-F745-9713-522C1AC36756}">
-  <dimension ref="B1:K15"/>
+  <dimension ref="B1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,162 +833,232 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="96" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="10" t="s">
-        <v>24</v>
+    <row r="8" spans="2:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="B8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>22</v>
+        <v>47</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="21">
-        <v>1</v>
+      <c r="H8" s="27">
+        <v>2</v>
       </c>
       <c r="I8" s="11">
         <v>2</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="21">
+        <v>1</v>
+      </c>
+      <c r="K8" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" s="23" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="B9" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="21">
+        <v>1</v>
+      </c>
+      <c r="I9" s="11">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21">
+        <v>1</v>
+      </c>
+      <c r="K9" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="21">
+        <v>1</v>
+      </c>
+      <c r="I10" s="11">
         <v>2</v>
       </c>
-      <c r="K8" s="9">
-        <f>SUM(H8:J8)</f>
+      <c r="J10" s="11">
+        <v>2</v>
+      </c>
+      <c r="K10" s="9">
+        <f>SUM(H10:J10)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="96" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+    <row r="11" spans="2:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="10" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="21">
-        <v>1</v>
-      </c>
-      <c r="I9" s="11">
+      <c r="F11" s="4"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="21">
+        <v>1</v>
+      </c>
+      <c r="I11" s="11">
         <v>2</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J11" s="11">
         <v>2</v>
       </c>
-      <c r="K9" s="9">
-        <f>SUM(H9:J9)</f>
+      <c r="K11" s="9">
+        <f>SUM(H11:J11)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="64" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15" t="s">
+    <row r="12" spans="2:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H12" s="9">
         <v>3</v>
       </c>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="2:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="2:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H13" s="9">
         <v>2</v>
       </c>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="2:11" ht="96" x14ac:dyDescent="0.2">
-      <c r="B12" s="13" t="s">
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="2:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="2:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="B15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="21">
-        <v>1</v>
-      </c>
-      <c r="I12" s="11">
+      <c r="H15" s="21">
+        <v>1</v>
+      </c>
+      <c r="I15" s="11">
         <v>2</v>
       </c>
-      <c r="J12" s="21">
-        <v>1</v>
-      </c>
-      <c r="K12" s="9">
-        <f>SUM(H12:J12)</f>
+      <c r="J15" s="21">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9">
+        <f>SUM(H15:J15)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="112" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+    <row r="16" spans="2:11" ht="112" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="21">
-        <v>1</v>
-      </c>
-      <c r="I13" s="21">
-        <v>1</v>
-      </c>
-      <c r="J13" s="21">
-        <v>1</v>
-      </c>
-      <c r="K13" s="9">
-        <f>SUM(H13:J13)</f>
+      <c r="H16" s="21">
+        <v>1</v>
+      </c>
+      <c r="I16" s="21">
+        <v>1</v>
+      </c>
+      <c r="J16" s="21">
+        <v>1</v>
+      </c>
+      <c r="K16" s="9">
+        <f>SUM(H16:J16)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+    <row r="17" spans="2:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="B17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H17" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="64" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+    <row r="18" spans="2:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H18" s="9">
         <v>2</v>
       </c>
     </row>

</xml_diff>